<commit_message>
ExampleMap - userstories - features
</commit_message>
<xml_diff>
--- a/docs/ExampleMap-TescoTest.xlsx
+++ b/docs/ExampleMap-TescoTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation Tanfolyam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DDBB3A-1633-4F7E-A616-CBE4CEB21EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED21A034-EC8C-4FBB-B232-43036FA61340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bejelentkezés" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Bejelentkezés</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Kijelentkezés</t>
-  </si>
-  <si>
-    <t>Be van jelentkezve</t>
   </si>
   <si>
     <r>
@@ -385,9 +382,6 @@
   </si>
   <si>
     <t>Van érvényes regisztráció, rossz e-mail/psw megadás</t>
-  </si>
-  <si>
-    <t>Be van jelentkezve, megkeresett egy terméket</t>
   </si>
   <si>
     <r>
@@ -469,50 +463,6 @@
       <rPr>
         <b/>
         <u/>
-        <sz val="16"/>
-        <color rgb="FF006100"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sikertelen kosárbahelyezés</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF006100"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- kivesz egy terméket a keresés teszt alapján
-- Keresés megvolt
-- Megjelent a: " Találatok erre “termékre”
-   Megjelenítve x termék y termékből"
-- ha x = 0, akkor
-=&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="16"/>
-        <color rgb="FF006100"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sajnos nem található a keresett termék raktárunkban</t>
-    </r>
-  </si>
-  <si>
-    <t>A Tesco főoldalon a jobb szélen megtalálható a Visszajelzés menüpont</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
         <sz val="14"/>
         <color rgb="FF006100"/>
         <rFont val="Calibri"/>
@@ -634,9 +584,6 @@
       </rPr>
       <t>Klikk a kérdőív x-ére, azaz bezárni</t>
     </r>
-  </si>
-  <si>
-    <t>Be van jelentkezve, kosárba tett egy terméket</t>
   </si>
   <si>
     <r>
@@ -750,12 +697,6 @@
     <t>Csak angol és magyar lehetőség van?</t>
   </si>
   <si>
-    <t>Angolul van -&gt; Magyarra vált</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Magyarul van -&gt; Angolra vált</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -853,6 +794,24 @@
   </si>
   <si>
     <t>Több elemet kellene tenni-venni?</t>
+  </si>
+  <si>
+    <t>Be van jelentkezve, létező termék kosárbatétele</t>
+  </si>
+  <si>
+    <t>Be van jelentkezve, kosárban lévő terméket töröl</t>
+  </si>
+  <si>
+    <t>A Tesco főoldalon a jobb szélen megtalálható a működő Visszajelzés menüpont</t>
+  </si>
+  <si>
+    <t>Be van jelentkezve és szabályosan kijelentkezik</t>
+  </si>
+  <si>
+    <t>Angolul van -&gt; Magyarra válthat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Magyarul van -&gt; Angolra válthat</t>
   </si>
 </sst>
 </file>
@@ -1159,9 +1118,6 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1171,6 +1127,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1492,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2FA75E-6386-442C-A390-0FDEBC53BE6E}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
@@ -1536,11 +1493,11 @@
     <row r="3" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:14" s="5" customFormat="1" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
@@ -1555,10 +1512,10 @@
     <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:14" ht="193.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
@@ -1579,10 +1536,10 @@
     </row>
     <row r="8" spans="1:14" ht="153.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="15"/>
+      <c r="A9" s="14"/>
     </row>
     <row r="10" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="16"/>
+      <c r="A10" s="15"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="12" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1599,234 +1556,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC736A94-E9A2-4471-87DD-6A03D55B005D}">
-  <dimension ref="A1:N14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="47.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="3" width="47.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="3" customWidth="1"/>
-    <col min="5" max="5" width="47.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="7" max="7" width="47.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="3" customWidth="1"/>
-    <col min="9" max="9" width="47.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="3" style="2" customWidth="1"/>
-    <col min="11" max="11" width="47.77734375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="3" style="2" customWidth="1"/>
-    <col min="13" max="13" width="47.77734375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="3" style="2" customWidth="1"/>
-    <col min="15" max="19" width="53.5546875" style="2" customWidth="1"/>
-    <col min="20" max="16384" width="9.21875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11"/>
-    </row>
-    <row r="2" spans="1:14" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="230.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="228.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="17"/>
-    </row>
-    <row r="10" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="16"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="12" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A9:A10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE39704-026C-4232-B3FD-A71A68D9EF54}">
-  <dimension ref="A1:N14"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="47.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="3" width="47.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="3" customWidth="1"/>
-    <col min="5" max="5" width="47.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="7" max="7" width="47.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="3" customWidth="1"/>
-    <col min="9" max="9" width="47.77734375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="3" style="2" customWidth="1"/>
-    <col min="11" max="11" width="47.77734375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="3" style="2" customWidth="1"/>
-    <col min="13" max="13" width="47.77734375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="3" style="2" customWidth="1"/>
-    <col min="15" max="19" width="53.5546875" style="2" customWidth="1"/>
-    <col min="20" max="16384" width="9.21875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11"/>
-    </row>
-    <row r="2" spans="1:14" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:14" ht="285" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="15"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="16"/>
-    </row>
-    <row r="10" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="12" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A8:A9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -1857,11 +1586,226 @@
       <c r="A1" s="11"/>
     </row>
     <row r="2" spans="1:14" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:14" s="5" customFormat="1" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:14" ht="230.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="228.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="16"/>
+    </row>
+    <row r="10" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="12" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:A10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE39704-026C-4232-B3FD-A71A68D9EF54}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="47.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="3" customWidth="1"/>
+    <col min="3" max="3" width="47.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="3" customWidth="1"/>
+    <col min="5" max="5" width="47.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3" customWidth="1"/>
+    <col min="7" max="7" width="47.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="9" width="47.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="3" style="2" customWidth="1"/>
+    <col min="11" max="11" width="47.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="3" style="2" customWidth="1"/>
+    <col min="13" max="13" width="47.77734375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="3" style="2" customWidth="1"/>
+    <col min="15" max="19" width="53.5546875" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9.21875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:14" s="5" customFormat="1" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:14" ht="285" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="14"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="12" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="47.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="3" customWidth="1"/>
+    <col min="3" max="3" width="47.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="3" customWidth="1"/>
+    <col min="5" max="5" width="47.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3" customWidth="1"/>
+    <col min="7" max="7" width="47.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="9" width="47.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="3" style="2" customWidth="1"/>
+    <col min="11" max="11" width="47.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="3" style="2" customWidth="1"/>
+    <col min="13" max="13" width="47.77734375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="3" style="2" customWidth="1"/>
+    <col min="15" max="19" width="53.5546875" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9.21875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1"/>
@@ -1873,7 +1817,7 @@
     <row r="3" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:14" s="5" customFormat="1" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4"/>
@@ -1890,9 +1834,9 @@
     <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:14" ht="251.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6"/>
+        <v>18</v>
+      </c>
+      <c r="C6" s="17"/>
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
       <c r="I6" s="1"/>
@@ -1911,10 +1855,10 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="17"/>
+      <c r="A8" s="16"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="17"/>
+      <c r="A9" s="16"/>
     </row>
     <row r="10" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1975,7 +1919,7 @@
     <row r="3" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:14" s="5" customFormat="1" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4"/>
@@ -1992,7 +1936,7 @@
     <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:14" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6"/>
       <c r="E6" s="1"/>
@@ -2013,10 +1957,10 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="17"/>
+      <c r="A8" s="16"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="17"/>
+      <c r="A9" s="16"/>
     </row>
     <row r="10" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -2037,7 +1981,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
@@ -2065,10 +2009,10 @@
     </row>
     <row r="2" spans="1:14" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="1"/>
@@ -2079,11 +2023,11 @@
     <row r="3" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:14" s="5" customFormat="1" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
@@ -2098,10 +2042,10 @@
     <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:14" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
@@ -2121,10 +2065,10 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="17"/>
+      <c r="A8" s="16"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="17"/>
+      <c r="A9" s="16"/>
     </row>
     <row r="10" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>